<commit_message>
first run on Japan data with KCOR
</commit_message>
<xml_diff>
--- a/data/japan/KCOR_summary.xlsx
+++ b/data/japan/KCOR_summary.xlsx
@@ -2096,7 +2096,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.2181</t>
+          <t>0.2182</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.351</t>
+          <t>0.352</t>
         </is>
       </c>
     </row>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.1793</t>
+          <t>0.1798</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.475</t>
+          <t>0.476</t>
         </is>
       </c>
     </row>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.3417</t>
+          <t>0.3418</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.2993</t>
+          <t>1.2967</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>12.993</t>
+          <t>12.967</t>
         </is>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.6948</t>
+          <t>0.6938</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>6.948</t>
+          <t>6.938</t>
         </is>
       </c>
     </row>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3.9441</t>
+          <t>3.9356</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2244,7 +2244,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>39.441</t>
+          <t>39.356</t>
         </is>
       </c>
     </row>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.2711</t>
+          <t>1.2669</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>12.711</t>
+          <t>12.669</t>
         </is>
       </c>
     </row>
@@ -2303,7 +2303,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.6140</t>
+          <t>0.3405</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2313,7 +2313,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>16.140</t>
+          <t>3.405</t>
         </is>
       </c>
     </row>
@@ -2344,17 +2344,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.2779</t>
+          <t>0.2785</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.179</t>
+          <t>0.180</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.431</t>
+          <t>0.432</t>
         </is>
       </c>
     </row>
@@ -2367,17 +2367,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.2538</t>
+          <t>0.2555</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.104</t>
+          <t>0.105</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.618</t>
+          <t>0.622</t>
         </is>
       </c>
     </row>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.3296</t>
+          <t>0.3297</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2436,7 +2436,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.3116</t>
+          <t>0.3109</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>3.116</t>
+          <t>3.109</t>
         </is>
       </c>
     </row>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.2925</t>
+          <t>0.2921</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2469,7 +2469,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2.925</t>
+          <t>2.921</t>
         </is>
       </c>
     </row>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.2378</t>
+          <t>1.2351</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2492,7 +2492,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>12.378</t>
+          <t>12.351</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.8061</t>
+          <t>0.8034</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2515,7 +2515,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>8.061</t>
+          <t>8.034</t>
         </is>
       </c>
     </row>
@@ -2551,7 +2551,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.9397</t>
+          <t>0.3242</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2561,7 +2561,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>19.397</t>
+          <t>3.242</t>
         </is>
       </c>
     </row>
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.4614</t>
+          <t>1.4622</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.227</t>
+          <t>1.228</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.741</t>
+          <t>1.742</t>
         </is>
       </c>
     </row>
@@ -2615,17 +2615,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.4158</t>
+          <t>1.4208</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.948</t>
+          <t>0.951</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2.114</t>
+          <t>2.122</t>
         </is>
       </c>
     </row>
@@ -2799,7 +2799,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.2018</t>
+          <t>0.9521</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2809,7 +2809,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>12.018</t>
+          <t>9.521</t>
         </is>
       </c>
     </row>
@@ -2840,7 +2840,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0.3668</t>
+          <t>0.3675</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -2850,7 +2850,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0.574</t>
+          <t>0.575</t>
         </is>
       </c>
     </row>
@@ -2863,17 +2863,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>0.3249</t>
+          <t>0.3270</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>0.133</t>
+          <t>0.134</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0.795</t>
+          <t>0.800</t>
         </is>
       </c>
     </row>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>0.6945</t>
+          <t>0.6946</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2932,7 +2932,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>0.1032</t>
+          <t>0.1030</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2942,7 +2942,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.032</t>
+          <t>1.030</t>
         </is>
       </c>
     </row>
@@ -2955,7 +2955,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.2365</t>
+          <t>0.2361</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2965,7 +2965,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2.365</t>
+          <t>2.361</t>
         </is>
       </c>
     </row>
@@ -2978,7 +2978,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>3.2552</t>
+          <t>3.2481</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>32.552</t>
+          <t>32.481</t>
         </is>
       </c>
     </row>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0.5058</t>
+          <t>0.5041</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3011,7 +3011,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>5.058</t>
+          <t>5.041</t>
         </is>
       </c>
     </row>
@@ -3088,17 +3088,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.5264</t>
+          <t>1.5274</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.261</t>
+          <t>1.262</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.848</t>
+          <t>1.849</t>
         </is>
       </c>
     </row>
@@ -3111,17 +3111,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.8123</t>
+          <t>1.8186</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.201</t>
+          <t>1.205</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2.735</t>
+          <t>2.745</t>
         </is>
       </c>
     </row>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.0323</t>
+          <t>1.0324</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.3628</t>
+          <t>0.3630</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.541</t>
+          <t>0.542</t>
         </is>
       </c>
     </row>
@@ -3664,7 +3664,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2.5748</t>
+          <t>2.0193</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3674,7 +3674,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>25.748</t>
+          <t>20.193</t>
         </is>
       </c>
     </row>
@@ -3687,7 +3687,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2.5028</t>
+          <t>2.4028</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3697,7 +3697,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>25.028</t>
+          <t>24.028</t>
         </is>
       </c>
     </row>
@@ -3733,7 +3733,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2.0173</t>
+          <t>2.0023</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3743,7 +3743,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>20.173</t>
+          <t>20.023</t>
         </is>
       </c>
     </row>
@@ -3756,7 +3756,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.1306</t>
+          <t>1.1248</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -3766,7 +3766,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>11.306</t>
+          <t>11.248</t>
         </is>
       </c>
     </row>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.7499</t>
+          <t>0.7501</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.990</t>
+          <t>1.991</t>
         </is>
       </c>
     </row>
@@ -3802,7 +3802,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.3694</t>
+          <t>0.3695</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.2279</t>
+          <t>0.2281</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3835,7 +3835,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.389</t>
+          <t>0.390</t>
         </is>
       </c>
     </row>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.4534</t>
+          <t>0.7480</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>4.534</t>
+          <t>7.480</t>
         </is>
       </c>
     </row>
@@ -3889,12 +3889,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.4762</t>
+          <t>0.4764</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.324</t>
+          <t>0.325</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -3912,7 +3912,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>5.5259</t>
+          <t>4.3084</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -3922,7 +3922,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>55.259</t>
+          <t>43.084</t>
         </is>
       </c>
     </row>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2.5552</t>
+          <t>2.4531</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>25.552</t>
+          <t>24.531</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.3787</t>
+          <t>1.3684</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>13.787</t>
+          <t>13.684</t>
         </is>
       </c>
     </row>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.3651</t>
+          <t>0.3632</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -4014,7 +4014,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3.651</t>
+          <t>3.632</t>
         </is>
       </c>
     </row>
@@ -4027,7 +4027,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.6681</t>
+          <t>0.6683</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -4050,7 +4050,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.6025</t>
+          <t>0.6028</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -4073,7 +4073,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.3212</t>
+          <t>0.3214</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -4083,7 +4083,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.542</t>
+          <t>0.543</t>
         </is>
       </c>
     </row>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.0877</t>
+          <t>0.2409</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.877</t>
+          <t>2.409</t>
         </is>
       </c>
     </row>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.9597</t>
+          <t>0.9588</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -4147,7 +4147,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.219</t>
+          <t>1.218</t>
         </is>
       </c>
     </row>
@@ -4160,17 +4160,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.0078</t>
+          <t>1.0019</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.523</t>
+          <t>0.520</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.941</t>
+          <t>1.929</t>
         </is>
       </c>
     </row>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.1934</t>
+          <t>0.3221</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -4354,7 +4354,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.934</t>
+          <t>3.221</t>
         </is>
       </c>
     </row>
@@ -4385,7 +4385,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0.4183</t>
+          <t>0.4185</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -4395,7 +4395,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0.611</t>
+          <t>0.612</t>
         </is>
       </c>
     </row>
@@ -4408,7 +4408,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2.8104</t>
+          <t>2.1912</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>28.104</t>
+          <t>21.912</t>
         </is>
       </c>
     </row>
@@ -4431,7 +4431,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2.0946</t>
+          <t>2.0109</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -4441,7 +4441,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>20.946</t>
+          <t>20.109</t>
         </is>
       </c>
     </row>
@@ -4477,7 +4477,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>0.6508</t>
+          <t>0.6460</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>6.508</t>
+          <t>6.460</t>
         </is>
       </c>
     </row>
@@ -4500,7 +4500,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.2689</t>
+          <t>0.2676</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -4510,7 +4510,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2.689</t>
+          <t>2.676</t>
         </is>
       </c>
     </row>
@@ -4523,7 +4523,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0.5428</t>
+          <t>0.5429</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0.4805</t>
+          <t>0.4807</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0.911</t>
+          <t>0.912</t>
         </is>
       </c>
     </row>
@@ -4569,7 +4569,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.3193</t>
+          <t>0.3195</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4592,7 +4592,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.0897</t>
+          <t>0.2319</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4602,7 +4602,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.897</t>
+          <t>2.319</t>
         </is>
       </c>
     </row>
@@ -4633,17 +4633,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>0.7997</t>
+          <t>0.7990</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.634</t>
+          <t>0.633</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>1.008</t>
         </is>
       </c>
     </row>
@@ -4656,17 +4656,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.6134</t>
+          <t>0.6098</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.324</t>
+          <t>0.322</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.162</t>
+          <t>1.155</t>
         </is>
       </c>
     </row>
@@ -4840,7 +4840,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.1978</t>
+          <t>0.3100</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -4850,7 +4850,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.978</t>
+          <t>3.100</t>
         </is>
       </c>
     </row>
@@ -4881,17 +4881,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>0.8176</t>
+          <t>0.8195</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0.755</t>
+          <t>0.757</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>0.885</t>
+          <t>0.887</t>
         </is>
       </c>
     </row>
@@ -5088,17 +5088,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1.3759</t>
+          <t>1.4530</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>0.772</t>
+          <t>0.957</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2.453</t>
+          <t>2.206</t>
         </is>
       </c>
     </row>
@@ -5129,7 +5129,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>0.4018</t>
+          <t>0.4021</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -5152,7 +5152,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2.3690</t>
+          <t>1.8470</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -5162,7 +5162,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>23.690</t>
+          <t>18.470</t>
         </is>
       </c>
     </row>
@@ -5175,7 +5175,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>0.8431</t>
+          <t>0.8094</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -5185,7 +5185,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>8.431</t>
+          <t>8.094</t>
         </is>
       </c>
     </row>
@@ -5221,7 +5221,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>0.4509</t>
+          <t>0.4475</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -5231,7 +5231,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>4.509</t>
+          <t>4.475</t>
         </is>
       </c>
     </row>
@@ -5244,7 +5244,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>0.3173</t>
+          <t>0.3157</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -5254,7 +5254,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>3.173</t>
+          <t>3.157</t>
         </is>
       </c>
     </row>
@@ -5267,7 +5267,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>0.4629</t>
+          <t>0.4630</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -5290,7 +5290,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>0.5177</t>
+          <t>0.5180</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -5300,7 +5300,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>0.997</t>
+          <t>0.998</t>
         </is>
       </c>
     </row>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>0.3021</t>
+          <t>0.3023</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -5336,7 +5336,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>0.1752</t>
+          <t>0.4643</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -5346,7 +5346,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>1.752</t>
+          <t>4.643</t>
         </is>
       </c>
     </row>
@@ -5377,17 +5377,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>0.9312</t>
+          <t>0.9302</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>0.738</t>
+          <t>0.737</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1.175</t>
+          <t>1.174</t>
         </is>
       </c>
     </row>
@@ -5400,17 +5400,17 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>0.9376</t>
+          <t>0.9320</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>0.498</t>
+          <t>0.495</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1.765</t>
+          <t>1.755</t>
         </is>
       </c>
     </row>
@@ -5584,7 +5584,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>0.3864</t>
+          <t>0.6208</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -5594,7 +5594,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>3.864</t>
+          <t>6.208</t>
         </is>
       </c>
     </row>
@@ -5625,7 +5625,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>0.9497</t>
+          <t>0.9496</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -5832,7 +5832,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>1.9980</t>
+          <t>1.9275</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -5842,7 +5842,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>19.980</t>
+          <t>19.275</t>
         </is>
       </c>
     </row>
@@ -5873,7 +5873,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>1.1641</t>
+          <t>1.1639</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -6080,7 +6080,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>1.9535</t>
+          <t>2.0025</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -6090,7 +6090,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>19.535</t>
+          <t>20.025</t>
         </is>
       </c>
     </row>

</xml_diff>